<commit_message>
refactor: migrate supporting CAF as a pacakge
</commit_message>
<xml_diff>
--- a/formulas.xlsx
+++ b/formulas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac/Downloads/cif-filter-featurizer-sorter-matcher-v5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac/Downloads/dev/oliynyk/composition-analyzer-featurizer/composition-analyzer-featurizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD30D25-854E-0D43-BCCF-86288A315D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6478C6-7C2C-0E4C-93CB-5B4CA99C5C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="660" windowWidth="19940" windowHeight="15980" xr2:uid="{AFAA846F-C9BE-0C44-872E-0A64BC1D6AC0}"/>
   </bookViews>
@@ -52,10 +52,10 @@
     <t>NdSi2</t>
   </si>
   <si>
-    <t>Th2Os</t>
+    <t>ThOs</t>
   </si>
   <si>
-    <t>Sn5Co2</t>
+    <t>YNdThSi2</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -462,12 +462,12 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -522,6 +522,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="842fee2d-b2cc-439f-a35b-e2ba2c54f32c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d103ac1e-cf17-436c-9a57-322643758598">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A76FEEB05DCAB449B725E81C3EC4FD4C" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9716df232e68d7c5a6e047c882f3a94b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d103ac1e-cf17-436c-9a57-322643758598" xmlns:ns3="842fee2d-b2cc-439f-a35b-e2ba2c54f32c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="152469c0b077a79ee0ff830005b6cb17" ns2:_="" ns3:_="">
     <xsd:import namespace="d103ac1e-cf17-436c-9a57-322643758598"/>
@@ -750,27 +770,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="842fee2d-b2cc-439f-a35b-e2ba2c54f32c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d103ac1e-cf17-436c-9a57-322643758598">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85B1AA1-687D-46E9-94CB-354533AF2EE4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9122F342-36C7-4695-B3C9-8773EFE605B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="842fee2d-b2cc-439f-a35b-e2ba2c54f32c"/>
+    <ds:schemaRef ds:uri="d103ac1e-cf17-436c-9a57-322643758598"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27B2AA21-DCC9-41AD-94F8-483DE1FFBEF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -787,23 +806,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9122F342-36C7-4695-B3C9-8773EFE605B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="842fee2d-b2cc-439f-a35b-e2ba2c54f32c"/>
-    <ds:schemaRef ds:uri="d103ac1e-cf17-436c-9a57-322643758598"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85B1AA1-687D-46E9-94CB-354533AF2EE4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>